<commit_message>
Working forms to create and implement salary request
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30329BFF-FE91-41CA-B04C-C9BA2D13CE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858D94C0-C246-403C-8331-231A752BCE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
           </rPr>
-          <t>jx:area(lastCell="N6")</t>
+          <t>jx:area(lastCell="R6")</t>
         </r>
       </text>
     </comment>
@@ -71,7 +71,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
           </rPr>
-          <t>jx:each(items="requests" var="r" lastCell="N6" orderBy="createdAt")</t>
+          <t>jx:each(items="requests" var="r" lastCell="R6" orderBy="createdAt")</t>
         </r>
       </text>
     </comment>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Выгрузка запросов на повышение или бонус</t>
   </si>
@@ -124,15 +124,9 @@
     <t>Причина запроса</t>
   </si>
   <si>
-    <t>Создано</t>
-  </si>
-  <si>
     <t>Результат</t>
   </si>
   <si>
-    <t>Реалиованная сумма в рублях</t>
-  </si>
-  <si>
     <t>Реализовано в периоде</t>
   </si>
   <si>
@@ -160,21 +154,12 @@
     <t>${r.type}</t>
   </si>
   <si>
-    <t>${r.reqSalaryIncrease}</t>
-  </si>
-  <si>
     <t>${r.reqReason}</t>
   </si>
   <si>
-    <t>${r.createdBy}</t>
-  </si>
-  <si>
     <t>${r.implState}</t>
   </si>
   <si>
-    <t>${r.implSalaryIncrease}</t>
-  </si>
-  <si>
     <t>${r.implIncreaseStartPeriod}</t>
   </si>
   <si>
@@ -191,6 +176,45 @@
   </si>
   <si>
     <t>${exportedAt} (${exportedBy})</t>
+  </si>
+  <si>
+    <t>Текущая заработная плата</t>
+  </si>
+  <si>
+    <t>Итоговая сумма</t>
+  </si>
+  <si>
+    <t>Итоговое изменение на</t>
+  </si>
+  <si>
+    <t>${r.currentSalaryAmount}</t>
+  </si>
+  <si>
+    <t>${r.reqPlannedSalaryAmount}</t>
+  </si>
+  <si>
+    <t>${r.implSalaryAmount}</t>
+  </si>
+  <si>
+    <t>Предполагаемая заработная плата после повышения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Источник финансирования (Бизнес аккаунт) </t>
+  </si>
+  <si>
+    <t>Бизнес Аккаунт</t>
+  </si>
+  <si>
+    <t>${r.budgetBusinessAccount}</t>
+  </si>
+  <si>
+    <t>${r.employeeBusinessAccount}</t>
+  </si>
+  <si>
+    <t>${r.implIncreaseAmount}</t>
+  </si>
+  <si>
+    <t>${r.reqIncreaseAmount}</t>
   </si>
 </sst>
 </file>
@@ -288,7 +312,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -311,11 +335,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -350,39 +442,65 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -398,27 +516,90 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -542,27 +723,63 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -579,6 +796,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -687,7 +905,6 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -712,7 +929,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -724,26 +945,60 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1053,32 +1308,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A5:N6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A5:N6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Позиция на проекте" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Тип" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Запрошенная сумма в рублях" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Причина запроса" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Создано" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Результат" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Реалиованная сумма в рублях" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Реализовано в периоде" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Новая позиция" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Реализовал" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Причина решения" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A5:R6" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A5:R6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Позиция на проекте" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{BAAD470C-6078-457E-BDFD-D2D54FF9B667}" name="Бизнес Аккаунт" dataDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{A372ED0E-D461-4DF3-916F-087E874A8A86}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Тип" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{4369F772-1B2A-45B1-BF44-11B5301A22B7}" name="Текущая заработная плата" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Запрошенная сумма в рублях" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{D6C42EED-0AD0-46D8-B960-F50A41CA22BB}" name="Предполагаемая заработная плата после повышения" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Причина запроса" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Результат" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Итоговое изменение на" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{D92B2A10-16DA-485C-B0D8-62B1A04E3205}" name="Итоговая сумма" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Реализовано в периоде" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Новая позиция" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Реализовал" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Причина решения" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1116,7 +1375,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1222,7 +1481,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1364,7 +1623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1372,34 +1631,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" customWidth="1"/>
+    <col min="18" max="18" width="31.85546875" customWidth="1"/>
     <col min="1013" max="1024" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1417,13 +1679,13 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1437,7 +1699,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -1457,31 +1719,35 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="6" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1489,103 +1755,127 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="J5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="M5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="8" t="s">
+    </row>
+    <row r="6" spans="1:18" s="9" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="E6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="H6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="M6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="F4:K4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+  <conditionalFormatting sqref="K6">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="L6">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ready to test functionality
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B8FD88-6A54-4214-9F30-CD95CC9E50B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9A6F9-2066-48A4-9A07-5D1507CA56A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="Q6")</t>
+          <t>jx:area(lastCell="R6")</t>
         </r>
       </text>
     </comment>
@@ -86,7 +86,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="requests" var="r" lastCell="Q6" orderBy="createdAt")</t>
+          <t>jx:each(items="requests" var="r" lastCell="R6" orderBy="createdAt")</t>
         </r>
       </text>
     </comment>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Выгрузка запросов на повышение ЗП</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Итоговая сумма бонуса</t>
+  </si>
+  <si>
+    <t>Запрошенная новая позиция</t>
+  </si>
+  <si>
+    <t>${r.reqNewPosition}</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -520,11 +526,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -601,9 +616,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -611,13 +623,59 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1387,9 +1445,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:Q6" totalsRowShown="0">
-  <autoFilter ref="A5:Q6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:R6" totalsRowShown="0">
+  <autoFilter ref="A5:R6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта"/>
@@ -1399,9 +1457,10 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Текущая заработная плата"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Запрошенная сумма в рублях"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Предполагаемая заработная плата после повышения"/>
+    <tableColumn id="7" xr3:uid="{9525771F-12E0-44D5-A45B-F79FFF58682F}" name="Запрошенная новая позиция" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Причина запроса"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="23"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Итоговая сумма"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Реализовано в периоде"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Новая позиция"/>
@@ -1413,23 +1472,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}" name="Table3" displayName="Table3" ref="A5:N6" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}" name="Table3" displayName="Table3" ref="A5:N6" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A5:N6" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{DCD7D2F7-C761-4D94-B041-DFF0DC3D5262}" name="ФИО" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{192AA3E5-92C7-477F-8B90-EB692C09CFA2}" name="Позиция по штатному расписанию" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{5CB5A664-75BF-4982-B80B-FB53302AF7B9}" name="Название проекта" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{3FC8D68E-C792-4E6E-9599-581DCF101221}" name="Позиция на проекте" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{8FE3C2A4-2CC4-4278-B478-5AB254E1C7C3}" name="Бизнес Аккаунт" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{80D2B666-2367-4A6B-A4B2-11F9507B3564}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{457064D5-278B-4AD6-86B2-69BEC0529512}" name="Причина запроса" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{8389C689-0177-423A-81F3-6C4D5B4F2E06}" name="Результат" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{258DE890-F924-467F-B8D7-2149A27DD50A}" name="Реализовано в периоде" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{A60531B9-5065-482B-A622-68DF33DE688A}" name="Реализовал" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{2F4744D6-F822-4678-AFEF-2363DE89DA81}" name="Причина решения" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{DCD7D2F7-C761-4D94-B041-DFF0DC3D5262}" name="ФИО" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{192AA3E5-92C7-477F-8B90-EB692C09CFA2}" name="Позиция по штатному расписанию" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5CB5A664-75BF-4982-B80B-FB53302AF7B9}" name="Название проекта" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{3FC8D68E-C792-4E6E-9599-581DCF101221}" name="Позиция на проекте" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{8FE3C2A4-2CC4-4278-B478-5AB254E1C7C3}" name="Бизнес Аккаунт" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{80D2B666-2367-4A6B-A4B2-11F9507B3564}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{457064D5-278B-4AD6-86B2-69BEC0529512}" name="Причина запроса" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{8389C689-0177-423A-81F3-6C4D5B4F2E06}" name="Результат" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{258DE890-F924-467F-B8D7-2149A27DD50A}" name="Реализовано в периоде" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{A60531B9-5065-482B-A622-68DF33DE688A}" name="Реализовал" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{2F4744D6-F822-4678-AFEF-2363DE89DA81}" name="Причина решения" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1755,11 +1814,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <selection pane="topRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,17 +1833,18 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
-    <col min="13" max="13" width="25" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
     <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="31.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" customWidth="1"/>
+    <col min="18" max="18" width="37.5703125" customWidth="1"/>
     <col min="1012" max="1023" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1801,7 +1861,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1820,7 +1880,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -1839,7 +1899,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>5</v>
       </c>
@@ -1849,24 +1909,25 @@
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="26" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
     </row>
-    <row r="5" spans="1:17" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1895,31 +1956,34 @@
         <v>17</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
@@ -1947,28 +2011,31 @@
       <c r="I6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="R6" s="10" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1976,14 +2043,14 @@
   <mergeCells count="4">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:R4"/>
   </mergeCells>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="L6">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2078,28 +2145,28 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="29" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
       <c r="AMG4"/>
       <c r="AMH4"/>
       <c r="AMI4"/>
@@ -2209,10 +2276,10 @@
     <mergeCell ref="J4:N4"/>
   </mergeCells>
   <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Feature/salaray UI refactoring (#76)
Move salary request details and all actions to the separate page.
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B8FD88-6A54-4214-9F30-CD95CC9E50B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9A6F9-2066-48A4-9A07-5D1507CA56A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="Q6")</t>
+          <t>jx:area(lastCell="R6")</t>
         </r>
       </text>
     </comment>
@@ -86,7 +86,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="requests" var="r" lastCell="Q6" orderBy="createdAt")</t>
+          <t>jx:each(items="requests" var="r" lastCell="R6" orderBy="createdAt")</t>
         </r>
       </text>
     </comment>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Выгрузка запросов на повышение ЗП</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Итоговая сумма бонуса</t>
+  </si>
+  <si>
+    <t>Запрошенная новая позиция</t>
+  </si>
+  <si>
+    <t>${r.reqNewPosition}</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -520,11 +526,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -601,9 +616,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -611,13 +623,59 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1387,9 +1445,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:Q6" totalsRowShown="0">
-  <autoFilter ref="A5:Q6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:R6" totalsRowShown="0">
+  <autoFilter ref="A5:R6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта"/>
@@ -1399,9 +1457,10 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Текущая заработная плата"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Запрошенная сумма в рублях"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Предполагаемая заработная плата после повышения"/>
+    <tableColumn id="7" xr3:uid="{9525771F-12E0-44D5-A45B-F79FFF58682F}" name="Запрошенная новая позиция" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Причина запроса"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="23"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Итоговая сумма"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Реализовано в периоде"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Новая позиция"/>
@@ -1413,23 +1472,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}" name="Table3" displayName="Table3" ref="A5:N6" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}" name="Table3" displayName="Table3" ref="A5:N6" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A5:N6" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{DCD7D2F7-C761-4D94-B041-DFF0DC3D5262}" name="ФИО" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{192AA3E5-92C7-477F-8B90-EB692C09CFA2}" name="Позиция по штатному расписанию" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{5CB5A664-75BF-4982-B80B-FB53302AF7B9}" name="Название проекта" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{3FC8D68E-C792-4E6E-9599-581DCF101221}" name="Позиция на проекте" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{8FE3C2A4-2CC4-4278-B478-5AB254E1C7C3}" name="Бизнес Аккаунт" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{80D2B666-2367-4A6B-A4B2-11F9507B3564}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{457064D5-278B-4AD6-86B2-69BEC0529512}" name="Причина запроса" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{8389C689-0177-423A-81F3-6C4D5B4F2E06}" name="Результат" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{258DE890-F924-467F-B8D7-2149A27DD50A}" name="Реализовано в периоде" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{A60531B9-5065-482B-A622-68DF33DE688A}" name="Реализовал" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{2F4744D6-F822-4678-AFEF-2363DE89DA81}" name="Причина решения" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{DCD7D2F7-C761-4D94-B041-DFF0DC3D5262}" name="ФИО" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{192AA3E5-92C7-477F-8B90-EB692C09CFA2}" name="Позиция по штатному расписанию" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5CB5A664-75BF-4982-B80B-FB53302AF7B9}" name="Название проекта" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{3FC8D68E-C792-4E6E-9599-581DCF101221}" name="Позиция на проекте" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{8FE3C2A4-2CC4-4278-B478-5AB254E1C7C3}" name="Бизнес Аккаунт" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{80D2B666-2367-4A6B-A4B2-11F9507B3564}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{457064D5-278B-4AD6-86B2-69BEC0529512}" name="Причина запроса" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{8389C689-0177-423A-81F3-6C4D5B4F2E06}" name="Результат" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{258DE890-F924-467F-B8D7-2149A27DD50A}" name="Реализовано в периоде" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{A60531B9-5065-482B-A622-68DF33DE688A}" name="Реализовал" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{2F4744D6-F822-4678-AFEF-2363DE89DA81}" name="Причина решения" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1755,11 +1814,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <selection pane="topRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,17 +1833,18 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
-    <col min="13" max="13" width="25" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
     <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="31.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" customWidth="1"/>
+    <col min="18" max="18" width="37.5703125" customWidth="1"/>
     <col min="1012" max="1023" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1801,7 +1861,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1820,7 +1880,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -1839,7 +1899,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>5</v>
       </c>
@@ -1849,24 +1909,25 @@
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="26" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
     </row>
-    <row r="5" spans="1:17" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1895,31 +1956,34 @@
         <v>17</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
@@ -1947,28 +2011,31 @@
       <c r="I6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="R6" s="10" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1976,14 +2043,14 @@
   <mergeCells count="4">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:R4"/>
   </mergeCells>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="L6">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2078,28 +2145,28 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="29" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
       <c r="AMG4"/>
       <c r="AMH4"/>
       <c r="AMI4"/>
@@ -2209,10 +2276,10 @@
     <mergeCell ref="J4:N4"/>
   </mergeCells>
   <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add few columns to salary requests export excel
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9A6F9-2066-48A4-9A07-5D1507CA56A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C2F11D-F59E-4D9D-96CE-F1F6235E657C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Запросы" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="R6")</t>
+          <t>jx:area(lastCell="V6")</t>
         </r>
       </text>
     </comment>
@@ -86,7 +86,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="requests" var="r" lastCell="R6" orderBy="createdAt")</t>
+          <t>jx:each(items="requests" var="r" lastCell="V6" orderBy="createdAt")</t>
         </r>
       </text>
     </comment>
@@ -120,7 +120,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="N6")</t>
+          <t>jx:area(lastCell="Q6")</t>
         </r>
       </text>
     </comment>
@@ -144,7 +144,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="bonuses" var="r" lastCell="N6" orderBy="createdAt")</t>
+          <t>jx:each(items="bonuses" var="r" lastCell="Q6" orderBy="createdAt")</t>
         </r>
       </text>
     </comment>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <t>Выгрузка запросов на повышение ЗП</t>
   </si>
@@ -297,17 +297,42 @@
   </si>
   <si>
     <t>${r.reqNewPosition}</t>
+  </si>
+  <si>
+    <t>Дата трудоустройства</t>
+  </si>
+  <si>
+    <t>${r.dateOfEmployment}</t>
+  </si>
+  <si>
+    <t>Инициатор</t>
+  </si>
+  <si>
+    <t>${r.createdBy}</t>
+  </si>
+  <si>
+    <t>Примечание</t>
+  </si>
+  <si>
+    <t>${r.implComment}</t>
+  </si>
+  <si>
+    <t>${r.budgetExpectedFundingUntil}</t>
+  </si>
+  <si>
+    <t>Перспективы биллинга</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -393,6 +418,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -420,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -503,43 +535,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
         <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -559,22 +583,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -592,23 +601,32 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -616,66 +634,30 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Денежный" xfId="1" builtinId="4"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="49">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -727,10 +709,10 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -760,9 +742,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -795,9 +775,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -811,6 +789,39 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -827,12 +838,99 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -846,7 +944,67 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -865,9 +1023,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -900,79 +1056,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1005,9 +1089,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1037,12 +1119,9 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1072,9 +1151,8 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1085,42 +1163,37 @@
           <color auto="1"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1142,51 +1215,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1211,6 +1246,26 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1257,13 +1312,658 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
-      </font>
+        <sz val="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
         <b/>
-      </font>
+        <sz val="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1445,59 +2145,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:R6" totalsRowShown="0">
-  <autoFilter ref="A5:R6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Позиция на проекте"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Бизнес Аккаунт"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Источник финансирования (Бизнес аккаунт) "/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Текущая заработная плата"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Запрошенная сумма в рублях"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Предполагаемая заработная плата после повышения"/>
-    <tableColumn id="7" xr3:uid="{9525771F-12E0-44D5-A45B-F79FFF58682F}" name="Запрошенная новая позиция" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Причина запроса"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Итоговая сумма"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Реализовано в периоде"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Новая позиция"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Реализовал"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Причина решения"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:V6" totalsRowShown="0" dataDxfId="48">
+  <autoFilter ref="A5:V6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО" dataDxfId="47"/>
+    <tableColumn id="21" xr3:uid="{9644AB1D-8B9B-4DD0-AA09-3BD71355E614}" name="Дата трудоустройства" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Позиция на проекте" dataDxfId="43"/>
+    <tableColumn id="22" xr3:uid="{77E31913-8C61-402B-A710-ECC629AF9FEB}" name="Инициатор" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Бизнес Аккаунт" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="40"/>
+    <tableColumn id="24" xr3:uid="{55967294-D7F3-44A4-92EA-B0EE380E00BC}" name="Перспективы биллинга" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Текущая заработная плата" dataDxfId="38" dataCellStyle="Денежный"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Запрошенная сумма в рублях" dataDxfId="37" dataCellStyle="Денежный"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Предполагаемая заработная плата после повышения" dataDxfId="36" dataCellStyle="Денежный"/>
+    <tableColumn id="7" xr3:uid="{9525771F-12E0-44D5-A45B-F79FFF58682F}" name="Запрошенная новая позиция" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Причина запроса" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="32" dataCellStyle="Денежный"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Итоговая сумма" dataDxfId="31" dataCellStyle="Денежный"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Реализовано в периоде" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Новая позиция" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Реализовал" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Причина решения" dataDxfId="27"/>
+    <tableColumn id="23" xr3:uid="{AC039516-1D6E-4411-893D-346D19B4FA55}" name="Примечание" dataDxfId="26"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}" name="Table3" displayName="Table3" ref="A5:N6" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="A5:N6" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{DCD7D2F7-C761-4D94-B041-DFF0DC3D5262}" name="ФИО" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{192AA3E5-92C7-477F-8B90-EB692C09CFA2}" name="Позиция по штатному расписанию" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{5CB5A664-75BF-4982-B80B-FB53302AF7B9}" name="Название проекта" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{3FC8D68E-C792-4E6E-9599-581DCF101221}" name="Позиция на проекте" dataDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}" name="Table3" displayName="Table3" ref="A5:Q6" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A5:Q6" xr:uid="{205D32E8-4F05-44AD-8F9E-52EFD083C729}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{DCD7D2F7-C761-4D94-B041-DFF0DC3D5262}" name="ФИО" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{B7FD5947-BACF-43A8-BFCC-2005FFE4EB16}" name="Дата трудоустройства" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{192AA3E5-92C7-477F-8B90-EB692C09CFA2}" name="Позиция по штатному расписанию" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{5CB5A664-75BF-4982-B80B-FB53302AF7B9}" name="Название проекта" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{3FC8D68E-C792-4E6E-9599-581DCF101221}" name="Позиция на проекте" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{E7EFC67E-3C1D-4059-A2B0-6EE1316836E6}" name="Инициатор" dataDxfId="15"/>
     <tableColumn id="5" xr3:uid="{8FE3C2A4-2CC4-4278-B478-5AB254E1C7C3}" name="Бизнес Аккаунт" dataDxfId="14"/>
     <tableColumn id="6" xr3:uid="{80D2B666-2367-4A6B-A4B2-11F9507B3564}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="12" dataCellStyle="Денежный"/>
+    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="11" dataCellStyle="Денежный"/>
     <tableColumn id="9" xr3:uid="{457064D5-278B-4AD6-86B2-69BEC0529512}" name="Причина запроса" dataDxfId="10"/>
     <tableColumn id="10" xr3:uid="{8389C689-0177-423A-81F3-6C4D5B4F2E06}" name="Результат" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="8" dataCellStyle="Денежный"/>
     <tableColumn id="12" xr3:uid="{258DE890-F924-467F-B8D7-2149A27DD50A}" name="Реализовано в периоде" dataDxfId="7"/>
     <tableColumn id="13" xr3:uid="{A60531B9-5065-482B-A622-68DF33DE688A}" name="Реализовал" dataDxfId="6"/>
     <tableColumn id="14" xr3:uid="{2F4744D6-F822-4678-AFEF-2363DE89DA81}" name="Причина решения" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{1C842CC2-520E-42C5-831F-A71E4CCBC2D1}" name="Примечание" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1535,7 +2242,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -1641,7 +2348,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1814,37 +2521,41 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" customWidth="1"/>
     <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" customWidth="1"/>
-    <col min="18" max="18" width="37.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="24.28515625" customWidth="1"/>
+    <col min="20" max="20" width="16" customWidth="1"/>
+    <col min="21" max="21" width="24.85546875" customWidth="1"/>
+    <col min="22" max="22" width="28" customWidth="1"/>
     <col min="1012" max="1023" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1861,7 +2572,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1880,7 +2591,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -1899,167 +2610,195 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="31" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="31" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
     </row>
-    <row r="5" spans="1:18" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="I5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="T5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="U5" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="V5" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:22" s="9" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="H6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="I6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="K6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="L6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="M6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="N6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="O6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="P6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="Q6" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="R6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="S6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="T6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="U6" s="19" t="s">
         <v>42</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="O4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="L6">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="O6">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2069,33 +2808,35 @@
   <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMM6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+      <selection pane="topRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="21.140625" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" customWidth="1"/>
     <col min="13" max="13" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" customWidth="1"/>
+    <col min="16" max="16" width="28" customWidth="1"/>
+    <col min="17" max="17" width="35.85546875" customWidth="1"/>
     <col min="1009" max="1024" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1027" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>43</v>
@@ -2110,7 +2851,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -2127,7 +2868,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -2144,142 +2885,163 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:1027" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="30"/>
       <c r="AMG4"/>
       <c r="AMH4"/>
       <c r="AMI4"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:1027" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="H5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="I5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="J5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="K5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="L5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="M5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="N5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="O5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="P5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AMG5"/>
-      <c r="AMH5"/>
-      <c r="AMI5"/>
+      <c r="Q5" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="AMJ5"/>
+      <c r="AMK5"/>
+      <c r="AML5"/>
+      <c r="AMM5"/>
     </row>
-    <row r="6" spans="1:1024" s="12" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:1027" s="9" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="F6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="H6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="I6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="J6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="K6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="L6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="M6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="N6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="O6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="P6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AMG6"/>
-      <c r="AMH6"/>
-      <c r="AMI6"/>
+      <c r="Q6" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="AMJ6"/>
+      <c r="AMK6"/>
+      <c r="AML6"/>
+      <c r="AMM6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="L4:Q4"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="F4:K4"/>
   </mergeCells>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="L6">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Реализован"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Отклонён"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add update impl text to export
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_salary_requests_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C2F11D-F59E-4D9D-96CE-F1F6235E657C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A3518-D42B-4B31-A2CD-B0BE905601E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="V6")</t>
+          <t>jx:area(lastCell="W6")</t>
         </r>
       </text>
     </comment>
@@ -86,7 +86,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="requests" var="r" lastCell="V6" orderBy="createdAt")</t>
+          <t>jx:each(items="requests" var="r" lastCell="W6" orderBy="employee")</t>
         </r>
       </text>
     </comment>
@@ -144,7 +144,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="bonuses" var="r" lastCell="Q6" orderBy="createdAt")</t>
+          <t>jx:each(items="bonuses" var="r" lastCell="Q6" orderBy="employee")</t>
         </r>
       </text>
     </comment>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>Выгрузка запросов на повышение ЗП</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>Перспективы биллинга</t>
+  </si>
+  <si>
+    <t>Сообщение об изменениях</t>
+  </si>
+  <si>
+    <t>${r.implIncreaseText}</t>
   </si>
 </sst>
 </file>
@@ -328,9 +334,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -561,9 +567,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -573,7 +579,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -604,10 +610,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,14 +625,20 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -654,10 +666,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Денежный" xfId="1" builtinId="4"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="50">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -838,7 +850,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -927,7 +939,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -960,7 +972,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1183,7 +1195,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1328,6 +1340,38 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1480,7 +1524,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1501,7 +1545,7 @@
         <family val="2"/>
         <charset val="204"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1553,7 +1597,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
+      <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* \-??\ [$₽-419]_-;_-@_-"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1613,7 +1657,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1644,7 +1688,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1675,7 +1719,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1706,7 +1750,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1921,7 +1965,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -2145,31 +2189,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:V6" totalsRowShown="0" dataDxfId="48">
-  <autoFilter ref="A5:V6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО" dataDxfId="47"/>
-    <tableColumn id="21" xr3:uid="{9644AB1D-8B9B-4DD0-AA09-3BD71355E614}" name="Дата трудоустройства" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Позиция на проекте" dataDxfId="43"/>
-    <tableColumn id="22" xr3:uid="{77E31913-8C61-402B-A710-ECC629AF9FEB}" name="Инициатор" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Бизнес Аккаунт" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="40"/>
-    <tableColumn id="24" xr3:uid="{55967294-D7F3-44A4-92EA-B0EE380E00BC}" name="Перспективы биллинга" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Текущая заработная плата" dataDxfId="38" dataCellStyle="Денежный"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Запрошенная сумма в рублях" dataDxfId="37" dataCellStyle="Денежный"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Предполагаемая заработная плата после повышения" dataDxfId="36" dataCellStyle="Денежный"/>
-    <tableColumn id="7" xr3:uid="{9525771F-12E0-44D5-A45B-F79FFF58682F}" name="Запрошенная новая позиция" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Причина запроса" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="32" dataCellStyle="Денежный"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Итоговая сумма" dataDxfId="31" dataCellStyle="Денежный"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Реализовано в периоде" dataDxfId="30"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Новая позиция" dataDxfId="29"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Реализовал" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Причина решения" dataDxfId="27"/>
-    <tableColumn id="23" xr3:uid="{AC039516-1D6E-4411-893D-346D19B4FA55}" name="Примечание" dataDxfId="26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица13" displayName="Таблица13" ref="A5:W6" totalsRowShown="0" dataDxfId="49">
+  <autoFilter ref="A5:W6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО" dataDxfId="48"/>
+    <tableColumn id="21" xr3:uid="{9644AB1D-8B9B-4DD0-AA09-3BD71355E614}" name="Дата трудоустройства" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Позиция по штатному расписанию" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Название проекта" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Позиция на проекте" dataDxfId="44"/>
+    <tableColumn id="22" xr3:uid="{77E31913-8C61-402B-A710-ECC629AF9FEB}" name="Инициатор" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Бизнес Аккаунт" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="41"/>
+    <tableColumn id="24" xr3:uid="{55967294-D7F3-44A4-92EA-B0EE380E00BC}" name="Перспективы биллинга" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Текущая заработная плата" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Запрошенная сумма в рублях" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Предполагаемая заработная плата после повышения" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{9525771F-12E0-44D5-A45B-F79FFF58682F}" name="Запрошенная новая позиция" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Причина запроса" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Результат" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Итоговое изменение на" dataDxfId="33"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Итоговая сумма" dataDxfId="32"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Реализовано в периоде" dataDxfId="31"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Новая позиция" dataDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Реализовал" dataDxfId="29"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Причина решения" dataDxfId="28"/>
+    <tableColumn id="23" xr3:uid="{AC039516-1D6E-4411-893D-346D19B4FA55}" name="Сообщение об изменениях" dataDxfId="27"/>
+    <tableColumn id="19" xr3:uid="{875B5ED8-83C0-4C33-A0D5-FA94658CDA01}" name="Примечание" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2187,11 +2232,11 @@
     <tableColumn id="17" xr3:uid="{E7EFC67E-3C1D-4059-A2B0-6EE1316836E6}" name="Инициатор" dataDxfId="15"/>
     <tableColumn id="5" xr3:uid="{8FE3C2A4-2CC4-4278-B478-5AB254E1C7C3}" name="Бизнес Аккаунт" dataDxfId="14"/>
     <tableColumn id="6" xr3:uid="{80D2B666-2367-4A6B-A4B2-11F9507B3564}" name="Источник финансирования (Бизнес аккаунт) " dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="12" dataCellStyle="Денежный"/>
-    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="11" dataCellStyle="Денежный"/>
+    <tableColumn id="7" xr3:uid="{BD707E8A-5B5C-4FB8-B195-6657E8D3ED1F}" name="Текущая заработная плата" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C0ACB597-F09F-4B12-82DA-24FAB94F1DDD}" name="Сумма бонуса" dataDxfId="11"/>
     <tableColumn id="9" xr3:uid="{457064D5-278B-4AD6-86B2-69BEC0529512}" name="Причина запроса" dataDxfId="10"/>
     <tableColumn id="10" xr3:uid="{8389C689-0177-423A-81F3-6C4D5B4F2E06}" name="Результат" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="8" dataCellStyle="Денежный"/>
+    <tableColumn id="11" xr3:uid="{3581A51A-B3DC-4B18-9277-BB4FCB5FF945}" name="Итоговая сумма бонуса" dataDxfId="8"/>
     <tableColumn id="12" xr3:uid="{258DE890-F924-467F-B8D7-2149A27DD50A}" name="Реализовано в периоде" dataDxfId="7"/>
     <tableColumn id="13" xr3:uid="{A60531B9-5065-482B-A622-68DF33DE688A}" name="Реализовал" dataDxfId="6"/>
     <tableColumn id="14" xr3:uid="{2F4744D6-F822-4678-AFEF-2363DE89DA81}" name="Причина решения" dataDxfId="5"/>
@@ -2202,9 +2247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2242,7 +2287,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -2348,7 +2393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2521,7 +2566,7 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -2551,11 +2596,12 @@
     <col min="19" max="19" width="24.28515625" customWidth="1"/>
     <col min="20" max="20" width="16" customWidth="1"/>
     <col min="21" max="21" width="24.85546875" customWidth="1"/>
-    <col min="22" max="22" width="28" customWidth="1"/>
+    <col min="22" max="22" width="41" customWidth="1"/>
+    <col min="23" max="23" width="23.42578125" customWidth="1"/>
     <col min="1012" max="1023" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2572,7 +2618,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -2591,7 +2637,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -2610,39 +2656,40 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="25" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="24"/>
     </row>
-    <row r="5" spans="1:22" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -2707,10 +2754,13 @@
         <v>25</v>
       </c>
       <c r="V5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="9" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" s="9" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>26</v>
       </c>
@@ -2775,15 +2825,17 @@
         <v>42</v>
       </c>
       <c r="V6" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="W6" s="19" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:N4"/>
-    <mergeCell ref="O4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="O6">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -2812,7 +2864,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L6" sqref="L6"/>
+      <selection pane="topRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2886,31 +2938,31 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:1027" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="28" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
       <c r="AMG4"/>
       <c r="AMH4"/>
       <c r="AMI4"/>

</xml_diff>